<commit_message>
casos de prueba viernes 10 de agosto
</commit_message>
<xml_diff>
--- a/1 Planeación de casos de pruebas CMMS(Recuperado automáticamente).xlsx
+++ b/1 Planeación de casos de pruebas CMMS(Recuperado automáticamente).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milenio\Desktop\testing\Pruebas\envios CMMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E487E8E5-13FA-49E3-8F22-C0B74F288DFF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BFB76D3A-3AF9-4350-BF30-A736B5D80D54}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1446,7 +1446,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1541,6 +1541,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="14">
     <fill>
@@ -1613,7 +1619,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2026,7 +2032,7 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2230,7 +2236,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2246,6 +2265,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2332,10 +2354,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -2751,11 +2776,11 @@
       </c>
       <c r="F4" s="3">
         <f>'Planeación detallada'!J138</f>
-        <v>0.58333333333333337</v>
+        <v>0.875</v>
       </c>
       <c r="G4" s="45">
         <f>'Planeación detallada'!K138</f>
-        <v>5.1100000000000003</v>
+        <v>7.6099999999999994</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2845,8 +2870,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:Z689"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C197" sqref="C197:C200"/>
+    <sheetView tabSelected="1" topLeftCell="A188" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="F225" sqref="F225:F228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2877,35 +2902,35 @@
     </row>
     <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="106"/>
-      <c r="H2" s="101">
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="107">
         <f>SUM(J6,J138,J238,J306,J334)/5</f>
-        <v>0.31666666666666671</v>
-      </c>
-      <c r="I2" s="101"/>
-      <c r="J2" s="101"/>
+        <v>0.375</v>
+      </c>
+      <c r="I2" s="107"/>
+      <c r="J2" s="107"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
-      <c r="B3" s="107"/>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="109"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="101"/>
+      <c r="B3" s="113"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="107"/>
+      <c r="I3" s="107"/>
+      <c r="J3" s="107"/>
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
       <c r="M3" s="14"/>
@@ -2973,7 +2998,7 @@
         <f>AVERAGE(J9:J136)</f>
         <v>1</v>
       </c>
-      <c r="K6" s="112">
+      <c r="K6" s="118">
         <f>SUM(F9:F136)</f>
         <v>8.7099999999999991</v>
       </c>
@@ -2992,7 +3017,7 @@
       <c r="H7" s="55"/>
       <c r="I7" s="55"/>
       <c r="J7" s="57"/>
-      <c r="K7" s="112"/>
+      <c r="K7" s="118"/>
       <c r="L7" s="14"/>
       <c r="M7" s="14"/>
     </row>
@@ -3035,7 +3060,7 @@
       <c r="B9" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="102" t="s">
+      <c r="C9" s="108" t="s">
         <v>45</v>
       </c>
       <c r="D9" s="25" t="s">
@@ -3061,7 +3086,7 @@
     <row r="10" spans="1:14" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="61"/>
       <c r="B10" s="69"/>
-      <c r="C10" s="103"/>
+      <c r="C10" s="109"/>
       <c r="D10" s="25" t="s">
         <v>50</v>
       </c>
@@ -3083,7 +3108,7 @@
     <row r="11" spans="1:14" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="61"/>
       <c r="B11" s="69"/>
-      <c r="C11" s="103"/>
+      <c r="C11" s="109"/>
       <c r="D11" s="25" t="s">
         <v>51</v>
       </c>
@@ -3105,7 +3130,7 @@
     <row r="12" spans="1:14" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="61"/>
       <c r="B12" s="69"/>
-      <c r="C12" s="103"/>
+      <c r="C12" s="109"/>
       <c r="D12" s="25" t="s">
         <v>52</v>
       </c>
@@ -3153,7 +3178,7 @@
     <row r="14" spans="1:14" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="61"/>
       <c r="B14" s="69"/>
-      <c r="C14" s="93"/>
+      <c r="C14" s="99"/>
       <c r="D14" s="25" t="s">
         <v>54</v>
       </c>
@@ -3175,7 +3200,7 @@
     <row r="15" spans="1:14" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="61"/>
       <c r="B15" s="69"/>
-      <c r="C15" s="93"/>
+      <c r="C15" s="99"/>
       <c r="D15" s="25" t="s">
         <v>55</v>
       </c>
@@ -3197,7 +3222,7 @@
     <row r="16" spans="1:14" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="61"/>
       <c r="B16" s="69"/>
-      <c r="C16" s="93"/>
+      <c r="C16" s="99"/>
       <c r="D16" s="25" t="s">
         <v>56</v>
       </c>
@@ -3381,7 +3406,7 @@
     <row r="24" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="61"/>
       <c r="B24" s="70"/>
-      <c r="C24" s="81"/>
+      <c r="C24" s="92"/>
       <c r="D24" s="25" t="s">
         <v>65</v>
       </c>
@@ -3431,9 +3456,9 @@
       </c>
     </row>
     <row r="26" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="91"/>
+      <c r="A26" s="97"/>
       <c r="B26" s="69"/>
-      <c r="C26" s="93"/>
+      <c r="C26" s="99"/>
       <c r="D26" s="25" t="s">
         <v>67</v>
       </c>
@@ -3453,9 +3478,9 @@
       </c>
     </row>
     <row r="27" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="91"/>
+      <c r="A27" s="97"/>
       <c r="B27" s="69"/>
-      <c r="C27" s="93"/>
+      <c r="C27" s="99"/>
       <c r="D27" s="25" t="s">
         <v>68</v>
       </c>
@@ -3475,9 +3500,9 @@
       </c>
     </row>
     <row r="28" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="91"/>
+      <c r="A28" s="97"/>
       <c r="B28" s="69"/>
-      <c r="C28" s="93"/>
+      <c r="C28" s="99"/>
       <c r="D28" s="25" t="s">
         <v>69</v>
       </c>
@@ -3497,7 +3522,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="91"/>
+      <c r="A29" s="97"/>
       <c r="B29" s="69"/>
       <c r="C29" s="66" t="s">
         <v>281</v>
@@ -3508,7 +3533,7 @@
       <c r="E29" s="19" t="s">
         <v>464</v>
       </c>
-      <c r="F29" s="82">
+      <c r="F29" s="87">
         <v>0.12</v>
       </c>
       <c r="G29" s="46"/>
@@ -3523,16 +3548,16 @@
       </c>
     </row>
     <row r="30" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="91"/>
+      <c r="A30" s="97"/>
       <c r="B30" s="69"/>
-      <c r="C30" s="96"/>
+      <c r="C30" s="102"/>
       <c r="D30" s="25" t="s">
         <v>71</v>
       </c>
       <c r="E30" s="19" t="s">
         <v>463</v>
       </c>
-      <c r="F30" s="83"/>
+      <c r="F30" s="88"/>
       <c r="G30" s="46"/>
       <c r="H30" s="30">
         <v>43283</v>
@@ -3545,16 +3570,16 @@
       </c>
     </row>
     <row r="31" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="91"/>
+      <c r="A31" s="97"/>
       <c r="B31" s="69"/>
-      <c r="C31" s="96"/>
+      <c r="C31" s="102"/>
       <c r="D31" s="25" t="s">
         <v>74</v>
       </c>
       <c r="E31" s="19" t="s">
         <v>466</v>
       </c>
-      <c r="F31" s="83"/>
+      <c r="F31" s="88"/>
       <c r="G31" s="46"/>
       <c r="H31" s="30">
         <v>43283</v>
@@ -3567,16 +3592,16 @@
       </c>
     </row>
     <row r="32" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="91"/>
+      <c r="A32" s="97"/>
       <c r="B32" s="69"/>
-      <c r="C32" s="96"/>
+      <c r="C32" s="102"/>
       <c r="D32" s="25" t="s">
         <v>75</v>
       </c>
       <c r="E32" s="19" t="s">
         <v>465</v>
       </c>
-      <c r="F32" s="84"/>
+      <c r="F32" s="89"/>
       <c r="G32" s="46"/>
       <c r="H32" s="30">
         <v>43283</v>
@@ -3589,7 +3614,7 @@
       </c>
     </row>
     <row r="33" spans="1:26" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="91"/>
+      <c r="A33" s="97"/>
       <c r="B33" s="69"/>
       <c r="C33" s="63" t="s">
         <v>282</v>
@@ -3600,7 +3625,7 @@
       <c r="E33" s="19" t="s">
         <v>464</v>
       </c>
-      <c r="F33" s="82">
+      <c r="F33" s="87">
         <v>0.3</v>
       </c>
       <c r="G33" s="46"/>
@@ -3615,7 +3640,7 @@
       </c>
     </row>
     <row r="34" spans="1:26" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="91"/>
+      <c r="A34" s="97"/>
       <c r="B34" s="69"/>
       <c r="C34" s="63"/>
       <c r="D34" s="25" t="s">
@@ -3624,7 +3649,7 @@
       <c r="E34" s="19" t="s">
         <v>463</v>
       </c>
-      <c r="F34" s="83"/>
+      <c r="F34" s="88"/>
       <c r="G34" s="46"/>
       <c r="H34" s="30">
         <v>43283</v>
@@ -3637,7 +3662,7 @@
       </c>
     </row>
     <row r="35" spans="1:26" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="91"/>
+      <c r="A35" s="97"/>
       <c r="B35" s="69"/>
       <c r="C35" s="63"/>
       <c r="D35" s="25" t="s">
@@ -3646,7 +3671,7 @@
       <c r="E35" s="19" t="s">
         <v>466</v>
       </c>
-      <c r="F35" s="83"/>
+      <c r="F35" s="88"/>
       <c r="G35" s="46"/>
       <c r="H35" s="30">
         <v>43283</v>
@@ -3659,7 +3684,7 @@
       </c>
     </row>
     <row r="36" spans="1:26" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="91"/>
+      <c r="A36" s="97"/>
       <c r="B36" s="69"/>
       <c r="C36" s="63"/>
       <c r="D36" s="25" t="s">
@@ -3668,7 +3693,7 @@
       <c r="E36" s="19" t="s">
         <v>465</v>
       </c>
-      <c r="F36" s="84"/>
+      <c r="F36" s="89"/>
       <c r="G36" s="9"/>
       <c r="H36" s="30">
         <v>43283</v>
@@ -3681,7 +3706,7 @@
       </c>
     </row>
     <row r="37" spans="1:26" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="91"/>
+      <c r="A37" s="97"/>
       <c r="B37" s="69"/>
       <c r="C37" s="63" t="s">
         <v>283</v>
@@ -3707,7 +3732,7 @@
       </c>
     </row>
     <row r="38" spans="1:26" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="91"/>
+      <c r="A38" s="97"/>
       <c r="B38" s="69"/>
       <c r="C38" s="63"/>
       <c r="D38" s="25" t="s">
@@ -3729,7 +3754,7 @@
       </c>
     </row>
     <row r="39" spans="1:26" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="91"/>
+      <c r="A39" s="97"/>
       <c r="B39" s="69"/>
       <c r="C39" s="63"/>
       <c r="D39" s="25" t="s">
@@ -3751,7 +3776,7 @@
       </c>
     </row>
     <row r="40" spans="1:26" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="91"/>
+      <c r="A40" s="97"/>
       <c r="B40" s="69"/>
       <c r="C40" s="63"/>
       <c r="D40" s="25" t="s">
@@ -3803,9 +3828,9 @@
       </c>
     </row>
     <row r="42" spans="1:26" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="91"/>
+      <c r="A42" s="97"/>
       <c r="B42" s="69"/>
-      <c r="C42" s="93"/>
+      <c r="C42" s="99"/>
       <c r="D42" s="25" t="s">
         <v>86</v>
       </c>
@@ -3826,9 +3851,9 @@
       <c r="Z42" s="27"/>
     </row>
     <row r="43" spans="1:26" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="91"/>
+      <c r="A43" s="97"/>
       <c r="B43" s="69"/>
-      <c r="C43" s="93"/>
+      <c r="C43" s="99"/>
       <c r="D43" s="25" t="s">
         <v>87</v>
       </c>
@@ -3848,9 +3873,9 @@
       </c>
     </row>
     <row r="44" spans="1:26" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="91"/>
+      <c r="A44" s="97"/>
       <c r="B44" s="69"/>
-      <c r="C44" s="93"/>
+      <c r="C44" s="99"/>
       <c r="D44" s="25" t="s">
         <v>88</v>
       </c>
@@ -3870,7 +3895,7 @@
       </c>
     </row>
     <row r="45" spans="1:26" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="91"/>
+      <c r="A45" s="97"/>
       <c r="B45" s="69"/>
       <c r="C45" s="66" t="s">
         <v>285</v>
@@ -3896,9 +3921,9 @@
       </c>
     </row>
     <row r="46" spans="1:26" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="91"/>
+      <c r="A46" s="97"/>
       <c r="B46" s="69"/>
-      <c r="C46" s="93"/>
+      <c r="C46" s="99"/>
       <c r="D46" s="25" t="s">
         <v>90</v>
       </c>
@@ -3918,9 +3943,9 @@
       </c>
     </row>
     <row r="47" spans="1:26" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="91"/>
+      <c r="A47" s="97"/>
       <c r="B47" s="69"/>
-      <c r="C47" s="93"/>
+      <c r="C47" s="99"/>
       <c r="D47" s="25" t="s">
         <v>91</v>
       </c>
@@ -3940,9 +3965,9 @@
       </c>
     </row>
     <row r="48" spans="1:26" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="91"/>
+      <c r="A48" s="97"/>
       <c r="B48" s="69"/>
-      <c r="C48" s="93"/>
+      <c r="C48" s="99"/>
       <c r="D48" s="25" t="s">
         <v>92</v>
       </c>
@@ -3962,7 +3987,7 @@
       </c>
     </row>
     <row r="49" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="91"/>
+      <c r="A49" s="97"/>
       <c r="B49" s="69"/>
       <c r="C49" s="78" t="s">
         <v>286</v>
@@ -3988,7 +4013,7 @@
       </c>
     </row>
     <row r="50" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="91"/>
+      <c r="A50" s="97"/>
       <c r="B50" s="69"/>
       <c r="C50" s="79"/>
       <c r="D50" s="25" t="s">
@@ -4010,7 +4035,7 @@
       </c>
     </row>
     <row r="51" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="91"/>
+      <c r="A51" s="97"/>
       <c r="B51" s="69"/>
       <c r="C51" s="79"/>
       <c r="D51" s="25" t="s">
@@ -4032,7 +4057,7 @@
       </c>
     </row>
     <row r="52" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="91"/>
+      <c r="A52" s="97"/>
       <c r="B52" s="69"/>
       <c r="C52" s="79"/>
       <c r="D52" s="25" t="s">
@@ -4054,7 +4079,7 @@
       </c>
     </row>
     <row r="53" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="91"/>
+      <c r="A53" s="97"/>
       <c r="B53" s="69"/>
       <c r="C53" s="63" t="s">
         <v>287</v>
@@ -4080,7 +4105,7 @@
       </c>
     </row>
     <row r="54" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="91"/>
+      <c r="A54" s="97"/>
       <c r="B54" s="69"/>
       <c r="C54" s="63"/>
       <c r="D54" s="25" t="s">
@@ -4102,9 +4127,9 @@
       </c>
     </row>
     <row r="55" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="91"/>
+      <c r="A55" s="97"/>
       <c r="B55" s="69"/>
-      <c r="C55" s="92"/>
+      <c r="C55" s="98"/>
       <c r="D55" s="25" t="s">
         <v>99</v>
       </c>
@@ -4124,9 +4149,9 @@
       </c>
     </row>
     <row r="56" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="91"/>
-      <c r="B56" s="90"/>
-      <c r="C56" s="92"/>
+      <c r="A56" s="97"/>
+      <c r="B56" s="96"/>
+      <c r="C56" s="98"/>
       <c r="D56" s="25" t="s">
         <v>100</v>
       </c>
@@ -4178,7 +4203,7 @@
     <row r="58" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="64"/>
       <c r="B58" s="69"/>
-      <c r="C58" s="96"/>
+      <c r="C58" s="102"/>
       <c r="D58" s="25" t="s">
         <v>102</v>
       </c>
@@ -4200,7 +4225,7 @@
     <row r="59" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="64"/>
       <c r="B59" s="69"/>
-      <c r="C59" s="96"/>
+      <c r="C59" s="102"/>
       <c r="D59" s="25" t="s">
         <v>103</v>
       </c>
@@ -4222,7 +4247,7 @@
     <row r="60" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="64"/>
       <c r="B60" s="69"/>
-      <c r="C60" s="110"/>
+      <c r="C60" s="116"/>
       <c r="D60" s="25" t="s">
         <v>104</v>
       </c>
@@ -4270,7 +4295,7 @@
     <row r="62" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="64"/>
       <c r="B62" s="69"/>
-      <c r="C62" s="96"/>
+      <c r="C62" s="102"/>
       <c r="D62" s="25" t="s">
         <v>106</v>
       </c>
@@ -4292,7 +4317,7 @@
     <row r="63" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="64"/>
       <c r="B63" s="69"/>
-      <c r="C63" s="96"/>
+      <c r="C63" s="102"/>
       <c r="D63" s="25" t="s">
         <v>107</v>
       </c>
@@ -4314,7 +4339,7 @@
     <row r="64" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="64"/>
       <c r="B64" s="69"/>
-      <c r="C64" s="111"/>
+      <c r="C64" s="117"/>
       <c r="D64" s="25" t="s">
         <v>108</v>
       </c>
@@ -4497,8 +4522,8 @@
     </row>
     <row r="72" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="64"/>
-      <c r="B72" s="90"/>
-      <c r="C72" s="81"/>
+      <c r="B72" s="96"/>
+      <c r="C72" s="92"/>
       <c r="D72" s="25" t="s">
         <v>116</v>
       </c>
@@ -4518,7 +4543,7 @@
       </c>
     </row>
     <row r="73" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="97" t="s">
+      <c r="A73" s="103" t="s">
         <v>15</v>
       </c>
       <c r="B73" s="66" t="s">
@@ -4548,9 +4573,9 @@
       </c>
     </row>
     <row r="74" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="98"/>
-      <c r="B74" s="96"/>
-      <c r="C74" s="96"/>
+      <c r="A74" s="104"/>
+      <c r="B74" s="102"/>
+      <c r="C74" s="102"/>
       <c r="D74" s="25" t="s">
         <v>118</v>
       </c>
@@ -4570,9 +4595,9 @@
       </c>
     </row>
     <row r="75" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="98"/>
-      <c r="B75" s="96"/>
-      <c r="C75" s="96"/>
+      <c r="A75" s="104"/>
+      <c r="B75" s="102"/>
+      <c r="C75" s="102"/>
       <c r="D75" s="25" t="s">
         <v>119</v>
       </c>
@@ -4592,9 +4617,9 @@
       </c>
     </row>
     <row r="76" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="100"/>
-      <c r="B76" s="93"/>
-      <c r="C76" s="93"/>
+      <c r="A76" s="106"/>
+      <c r="B76" s="99"/>
+      <c r="C76" s="99"/>
       <c r="D76" s="25" t="s">
         <v>120</v>
       </c>
@@ -4644,9 +4669,9 @@
       </c>
     </row>
     <row r="78" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="91"/>
+      <c r="A78" s="97"/>
       <c r="B78" s="69"/>
-      <c r="C78" s="93"/>
+      <c r="C78" s="99"/>
       <c r="D78" s="25" t="s">
         <v>124</v>
       </c>
@@ -4666,9 +4691,9 @@
       </c>
     </row>
     <row r="79" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="91"/>
+      <c r="A79" s="97"/>
       <c r="B79" s="69"/>
-      <c r="C79" s="93"/>
+      <c r="C79" s="99"/>
       <c r="D79" s="25" t="s">
         <v>125</v>
       </c>
@@ -4688,9 +4713,9 @@
       </c>
     </row>
     <row r="80" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="91"/>
+      <c r="A80" s="97"/>
       <c r="B80" s="69"/>
-      <c r="C80" s="93"/>
+      <c r="C80" s="99"/>
       <c r="D80" s="25" t="s">
         <v>126</v>
       </c>
@@ -4710,7 +4735,7 @@
       </c>
     </row>
     <row r="81" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="91"/>
+      <c r="A81" s="97"/>
       <c r="B81" s="69"/>
       <c r="C81" s="78" t="s">
         <v>294</v>
@@ -4736,7 +4761,7 @@
       </c>
     </row>
     <row r="82" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="91"/>
+      <c r="A82" s="97"/>
       <c r="B82" s="69"/>
       <c r="C82" s="79"/>
       <c r="D82" s="25" t="s">
@@ -4758,7 +4783,7 @@
       </c>
     </row>
     <row r="83" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="91"/>
+      <c r="A83" s="97"/>
       <c r="B83" s="69"/>
       <c r="C83" s="79"/>
       <c r="D83" s="25" t="s">
@@ -4780,7 +4805,7 @@
       </c>
     </row>
     <row r="84" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="91"/>
+      <c r="A84" s="97"/>
       <c r="B84" s="69"/>
       <c r="C84" s="79"/>
       <c r="D84" s="25" t="s">
@@ -4802,7 +4827,7 @@
       </c>
     </row>
     <row r="85" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="91"/>
+      <c r="A85" s="97"/>
       <c r="B85" s="69"/>
       <c r="C85" s="63" t="s">
         <v>295</v>
@@ -4828,7 +4853,7 @@
       </c>
     </row>
     <row r="86" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="91"/>
+      <c r="A86" s="97"/>
       <c r="B86" s="69"/>
       <c r="C86" s="63"/>
       <c r="D86" s="25" t="s">
@@ -4850,9 +4875,9 @@
       </c>
     </row>
     <row r="87" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="91"/>
+      <c r="A87" s="97"/>
       <c r="B87" s="69"/>
-      <c r="C87" s="92"/>
+      <c r="C87" s="98"/>
       <c r="D87" s="25" t="s">
         <v>133</v>
       </c>
@@ -4872,9 +4897,9 @@
       </c>
     </row>
     <row r="88" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="91"/>
-      <c r="B88" s="90"/>
-      <c r="C88" s="92"/>
+      <c r="A88" s="97"/>
+      <c r="B88" s="96"/>
+      <c r="C88" s="98"/>
       <c r="D88" s="25" t="s">
         <v>134</v>
       </c>
@@ -4924,9 +4949,9 @@
       </c>
     </row>
     <row r="90" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="91"/>
+      <c r="A90" s="97"/>
       <c r="B90" s="69"/>
-      <c r="C90" s="93"/>
+      <c r="C90" s="99"/>
       <c r="D90" s="25" t="s">
         <v>136</v>
       </c>
@@ -4946,9 +4971,9 @@
       </c>
     </row>
     <row r="91" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="91"/>
+      <c r="A91" s="97"/>
       <c r="B91" s="69"/>
-      <c r="C91" s="93"/>
+      <c r="C91" s="99"/>
       <c r="D91" s="25" t="s">
         <v>137</v>
       </c>
@@ -4968,9 +4993,9 @@
       </c>
     </row>
     <row r="92" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="91"/>
+      <c r="A92" s="97"/>
       <c r="B92" s="69"/>
-      <c r="C92" s="93"/>
+      <c r="C92" s="99"/>
       <c r="D92" s="25" t="s">
         <v>138</v>
       </c>
@@ -4990,7 +5015,7 @@
       </c>
     </row>
     <row r="93" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="91"/>
+      <c r="A93" s="97"/>
       <c r="B93" s="69"/>
       <c r="C93" s="66" t="s">
         <v>297</v>
@@ -5016,9 +5041,9 @@
       </c>
     </row>
     <row r="94" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="91"/>
+      <c r="A94" s="97"/>
       <c r="B94" s="69"/>
-      <c r="C94" s="93"/>
+      <c r="C94" s="99"/>
       <c r="D94" s="25" t="s">
         <v>140</v>
       </c>
@@ -5038,9 +5063,9 @@
       </c>
     </row>
     <row r="95" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="91"/>
+      <c r="A95" s="97"/>
       <c r="B95" s="69"/>
-      <c r="C95" s="93"/>
+      <c r="C95" s="99"/>
       <c r="D95" s="25" t="s">
         <v>141</v>
       </c>
@@ -5060,9 +5085,9 @@
       </c>
     </row>
     <row r="96" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="91"/>
+      <c r="A96" s="97"/>
       <c r="B96" s="69"/>
-      <c r="C96" s="93"/>
+      <c r="C96" s="99"/>
       <c r="D96" s="25" t="s">
         <v>142</v>
       </c>
@@ -5082,7 +5107,7 @@
       </c>
     </row>
     <row r="97" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="91"/>
+      <c r="A97" s="97"/>
       <c r="B97" s="69"/>
       <c r="C97" s="78" t="s">
         <v>298</v>
@@ -5108,7 +5133,7 @@
       </c>
     </row>
     <row r="98" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="91"/>
+      <c r="A98" s="97"/>
       <c r="B98" s="69"/>
       <c r="C98" s="79"/>
       <c r="D98" s="25" t="s">
@@ -5130,7 +5155,7 @@
       </c>
     </row>
     <row r="99" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="91"/>
+      <c r="A99" s="97"/>
       <c r="B99" s="69"/>
       <c r="C99" s="79"/>
       <c r="D99" s="25" t="s">
@@ -5152,7 +5177,7 @@
       </c>
     </row>
     <row r="100" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="91"/>
+      <c r="A100" s="97"/>
       <c r="B100" s="69"/>
       <c r="C100" s="79"/>
       <c r="D100" s="25" t="s">
@@ -5174,7 +5199,7 @@
       </c>
     </row>
     <row r="101" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="91"/>
+      <c r="A101" s="97"/>
       <c r="B101" s="69"/>
       <c r="C101" s="63" t="s">
         <v>299</v>
@@ -5200,7 +5225,7 @@
       </c>
     </row>
     <row r="102" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="91"/>
+      <c r="A102" s="97"/>
       <c r="B102" s="69"/>
       <c r="C102" s="63"/>
       <c r="D102" s="25" t="s">
@@ -5222,9 +5247,9 @@
       </c>
     </row>
     <row r="103" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="91"/>
+      <c r="A103" s="97"/>
       <c r="B103" s="69"/>
-      <c r="C103" s="92"/>
+      <c r="C103" s="98"/>
       <c r="D103" s="25" t="s">
         <v>152</v>
       </c>
@@ -5244,9 +5269,9 @@
       </c>
     </row>
     <row r="104" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="91"/>
-      <c r="B104" s="90"/>
-      <c r="C104" s="92"/>
+      <c r="A104" s="97"/>
+      <c r="B104" s="96"/>
+      <c r="C104" s="98"/>
       <c r="D104" s="25" t="s">
         <v>153</v>
       </c>
@@ -5296,9 +5321,9 @@
       </c>
     </row>
     <row r="106" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="91"/>
+      <c r="A106" s="97"/>
       <c r="B106" s="69"/>
-      <c r="C106" s="93"/>
+      <c r="C106" s="99"/>
       <c r="D106" s="25" t="s">
         <v>155</v>
       </c>
@@ -5318,9 +5343,9 @@
       </c>
     </row>
     <row r="107" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="91"/>
+      <c r="A107" s="97"/>
       <c r="B107" s="69"/>
-      <c r="C107" s="93"/>
+      <c r="C107" s="99"/>
       <c r="D107" s="25" t="s">
         <v>156</v>
       </c>
@@ -5340,9 +5365,9 @@
       </c>
     </row>
     <row r="108" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="91"/>
+      <c r="A108" s="97"/>
       <c r="B108" s="69"/>
-      <c r="C108" s="93"/>
+      <c r="C108" s="99"/>
       <c r="D108" s="25" t="s">
         <v>157</v>
       </c>
@@ -5362,7 +5387,7 @@
       </c>
     </row>
     <row r="109" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="91"/>
+      <c r="A109" s="97"/>
       <c r="B109" s="69"/>
       <c r="C109" s="63" t="s">
         <v>301</v>
@@ -5388,9 +5413,9 @@
       </c>
     </row>
     <row r="110" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="91"/>
+      <c r="A110" s="97"/>
       <c r="B110" s="69"/>
-      <c r="C110" s="92"/>
+      <c r="C110" s="98"/>
       <c r="D110" s="25" t="s">
         <v>279</v>
       </c>
@@ -5410,9 +5435,9 @@
       </c>
     </row>
     <row r="111" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="91"/>
+      <c r="A111" s="97"/>
       <c r="B111" s="69"/>
-      <c r="C111" s="92"/>
+      <c r="C111" s="98"/>
       <c r="D111" s="25" t="s">
         <v>161</v>
       </c>
@@ -5432,9 +5457,9 @@
       </c>
     </row>
     <row r="112" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="91"/>
+      <c r="A112" s="97"/>
       <c r="B112" s="69"/>
-      <c r="C112" s="92"/>
+      <c r="C112" s="98"/>
       <c r="D112" s="25" t="s">
         <v>162</v>
       </c>
@@ -5454,7 +5479,7 @@
       </c>
     </row>
     <row r="113" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="91"/>
+      <c r="A113" s="97"/>
       <c r="B113" s="69"/>
       <c r="C113" s="63" t="s">
         <v>302</v>
@@ -5480,7 +5505,7 @@
       </c>
     </row>
     <row r="114" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="91"/>
+      <c r="A114" s="97"/>
       <c r="B114" s="69"/>
       <c r="C114" s="63"/>
       <c r="D114" s="25" t="s">
@@ -5502,7 +5527,7 @@
       </c>
     </row>
     <row r="115" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="91"/>
+      <c r="A115" s="97"/>
       <c r="B115" s="69"/>
       <c r="C115" s="63"/>
       <c r="D115" s="25" t="s">
@@ -5524,7 +5549,7 @@
       </c>
     </row>
     <row r="116" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="91"/>
+      <c r="A116" s="97"/>
       <c r="B116" s="69"/>
       <c r="C116" s="63"/>
       <c r="D116" s="25" t="s">
@@ -5546,7 +5571,7 @@
       </c>
     </row>
     <row r="117" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="91"/>
+      <c r="A117" s="97"/>
       <c r="B117" s="69"/>
       <c r="C117" s="63" t="s">
         <v>303</v>
@@ -5572,7 +5597,7 @@
       </c>
     </row>
     <row r="118" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="91"/>
+      <c r="A118" s="97"/>
       <c r="B118" s="69"/>
       <c r="C118" s="63"/>
       <c r="D118" s="25" t="s">
@@ -5594,7 +5619,7 @@
       </c>
     </row>
     <row r="119" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="91"/>
+      <c r="A119" s="97"/>
       <c r="B119" s="69"/>
       <c r="C119" s="63"/>
       <c r="D119" s="25" t="s">
@@ -5616,8 +5641,8 @@
       </c>
     </row>
     <row r="120" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="91"/>
-      <c r="B120" s="90"/>
+      <c r="A120" s="97"/>
+      <c r="B120" s="96"/>
       <c r="C120" s="63"/>
       <c r="D120" s="25" t="s">
         <v>170</v>
@@ -5653,7 +5678,7 @@
       <c r="E121" s="24" t="s">
         <v>464</v>
       </c>
-      <c r="F121" s="82">
+      <c r="F121" s="87">
         <v>0.4</v>
       </c>
       <c r="G121" s="46"/>
@@ -5668,16 +5693,16 @@
       </c>
     </row>
     <row r="122" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="91"/>
+      <c r="A122" s="97"/>
       <c r="B122" s="69"/>
-      <c r="C122" s="92"/>
+      <c r="C122" s="98"/>
       <c r="D122" s="25" t="s">
         <v>173</v>
       </c>
       <c r="E122" s="24" t="s">
         <v>463</v>
       </c>
-      <c r="F122" s="83"/>
+      <c r="F122" s="88"/>
       <c r="G122" s="46"/>
       <c r="H122" s="30">
         <v>43283</v>
@@ -5690,16 +5715,16 @@
       </c>
     </row>
     <row r="123" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="91"/>
+      <c r="A123" s="97"/>
       <c r="B123" s="69"/>
-      <c r="C123" s="92"/>
+      <c r="C123" s="98"/>
       <c r="D123" s="25" t="s">
         <v>174</v>
       </c>
       <c r="E123" s="24" t="s">
         <v>466</v>
       </c>
-      <c r="F123" s="83"/>
+      <c r="F123" s="88"/>
       <c r="G123" s="46"/>
       <c r="H123" s="30">
         <v>43283</v>
@@ -5712,16 +5737,16 @@
       </c>
     </row>
     <row r="124" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="91"/>
+      <c r="A124" s="97"/>
       <c r="B124" s="69"/>
-      <c r="C124" s="92"/>
+      <c r="C124" s="98"/>
       <c r="D124" s="25" t="s">
         <v>175</v>
       </c>
       <c r="E124" s="24" t="s">
         <v>465</v>
       </c>
-      <c r="F124" s="84"/>
+      <c r="F124" s="89"/>
       <c r="G124" s="9"/>
       <c r="H124" s="30">
         <v>43283</v>
@@ -5734,7 +5759,7 @@
       </c>
     </row>
     <row r="125" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="91"/>
+      <c r="A125" s="97"/>
       <c r="B125" s="69"/>
       <c r="C125" s="63" t="s">
         <v>305</v>
@@ -5745,7 +5770,7 @@
       <c r="E125" s="24" t="s">
         <v>464</v>
       </c>
-      <c r="F125" s="82">
+      <c r="F125" s="87">
         <v>0.3</v>
       </c>
       <c r="G125" s="46"/>
@@ -5760,16 +5785,16 @@
       </c>
     </row>
     <row r="126" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="91"/>
+      <c r="A126" s="97"/>
       <c r="B126" s="69"/>
-      <c r="C126" s="92"/>
+      <c r="C126" s="98"/>
       <c r="D126" s="25" t="s">
         <v>177</v>
       </c>
       <c r="E126" s="24" t="s">
         <v>463</v>
       </c>
-      <c r="F126" s="83"/>
+      <c r="F126" s="88"/>
       <c r="G126" s="46"/>
       <c r="H126" s="30">
         <v>43283</v>
@@ -5782,16 +5807,16 @@
       </c>
     </row>
     <row r="127" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="91"/>
+      <c r="A127" s="97"/>
       <c r="B127" s="69"/>
-      <c r="C127" s="92"/>
+      <c r="C127" s="98"/>
       <c r="D127" s="25" t="s">
         <v>178</v>
       </c>
       <c r="E127" s="24" t="s">
         <v>466</v>
       </c>
-      <c r="F127" s="83"/>
+      <c r="F127" s="88"/>
       <c r="G127" s="46"/>
       <c r="H127" s="30">
         <v>43283</v>
@@ -5804,16 +5829,16 @@
       </c>
     </row>
     <row r="128" spans="1:10" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="91"/>
+      <c r="A128" s="97"/>
       <c r="B128" s="69"/>
-      <c r="C128" s="92"/>
+      <c r="C128" s="98"/>
       <c r="D128" s="25" t="s">
         <v>179</v>
       </c>
       <c r="E128" s="24" t="s">
         <v>465</v>
       </c>
-      <c r="F128" s="84"/>
+      <c r="F128" s="89"/>
       <c r="G128" s="46"/>
       <c r="H128" s="30">
         <v>43283</v>
@@ -5826,7 +5851,7 @@
       </c>
     </row>
     <row r="129" spans="1:14" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="91"/>
+      <c r="A129" s="97"/>
       <c r="B129" s="69"/>
       <c r="C129" s="63" t="s">
         <v>306</v>
@@ -5837,7 +5862,7 @@
       <c r="E129" s="24" t="s">
         <v>464</v>
       </c>
-      <c r="F129" s="82">
+      <c r="F129" s="87">
         <v>0.32</v>
       </c>
       <c r="G129" s="9"/>
@@ -5852,7 +5877,7 @@
       </c>
     </row>
     <row r="130" spans="1:14" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="91"/>
+      <c r="A130" s="97"/>
       <c r="B130" s="69"/>
       <c r="C130" s="63"/>
       <c r="D130" s="25" t="s">
@@ -5861,7 +5886,7 @@
       <c r="E130" s="24" t="s">
         <v>463</v>
       </c>
-      <c r="F130" s="83"/>
+      <c r="F130" s="88"/>
       <c r="G130" s="46"/>
       <c r="H130" s="30">
         <v>43283</v>
@@ -5874,7 +5899,7 @@
       </c>
     </row>
     <row r="131" spans="1:14" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="91"/>
+      <c r="A131" s="97"/>
       <c r="B131" s="69"/>
       <c r="C131" s="63"/>
       <c r="D131" s="25" t="s">
@@ -5883,7 +5908,7 @@
       <c r="E131" s="24" t="s">
         <v>466</v>
       </c>
-      <c r="F131" s="83"/>
+      <c r="F131" s="88"/>
       <c r="G131" s="46"/>
       <c r="H131" s="30">
         <v>43283</v>
@@ -5896,7 +5921,7 @@
       </c>
     </row>
     <row r="132" spans="1:14" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="91"/>
+      <c r="A132" s="97"/>
       <c r="B132" s="69"/>
       <c r="C132" s="63"/>
       <c r="D132" s="25" t="s">
@@ -5905,7 +5930,7 @@
       <c r="E132" s="24" t="s">
         <v>465</v>
       </c>
-      <c r="F132" s="84"/>
+      <c r="F132" s="89"/>
       <c r="G132" s="8"/>
       <c r="H132" s="30">
         <v>43283</v>
@@ -5918,7 +5943,7 @@
       </c>
     </row>
     <row r="133" spans="1:14" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="91"/>
+      <c r="A133" s="97"/>
       <c r="B133" s="69"/>
       <c r="C133" s="63" t="s">
         <v>307</v>
@@ -5944,7 +5969,7 @@
       </c>
     </row>
     <row r="134" spans="1:14" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="91"/>
+      <c r="A134" s="97"/>
       <c r="B134" s="69"/>
       <c r="C134" s="63"/>
       <c r="D134" s="25" t="s">
@@ -5966,9 +5991,9 @@
       </c>
     </row>
     <row r="135" spans="1:14" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="91"/>
+      <c r="A135" s="97"/>
       <c r="B135" s="69"/>
-      <c r="C135" s="92"/>
+      <c r="C135" s="98"/>
       <c r="D135" s="25" t="s">
         <v>187</v>
       </c>
@@ -5988,9 +6013,9 @@
       </c>
     </row>
     <row r="136" spans="1:14" s="28" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="91"/>
+      <c r="A136" s="97"/>
       <c r="B136" s="70"/>
-      <c r="C136" s="92"/>
+      <c r="C136" s="98"/>
       <c r="D136" s="25" t="s">
         <v>188</v>
       </c>
@@ -6055,11 +6080,11 @@
       </c>
       <c r="J138" s="56">
         <f>AVERAGE(J141:J236)</f>
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="K138" s="112">
+        <v>0.875</v>
+      </c>
+      <c r="K138" s="118">
         <f>SUM(F141:F236)</f>
-        <v>5.1100000000000003</v>
+        <v>7.6099999999999994</v>
       </c>
       <c r="L138" s="8"/>
       <c r="M138" s="12"/>
@@ -6076,7 +6101,7 @@
       <c r="H139" s="55"/>
       <c r="I139" s="55"/>
       <c r="J139" s="57"/>
-      <c r="K139" s="112"/>
+      <c r="K139" s="118"/>
       <c r="L139" s="14"/>
       <c r="M139" s="14"/>
       <c r="N139" s="14"/>
@@ -6469,8 +6494,8 @@
     </row>
     <row r="156" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="65"/>
-      <c r="B156" s="90"/>
-      <c r="C156" s="81"/>
+      <c r="B156" s="96"/>
+      <c r="C156" s="92"/>
       <c r="D156" s="10" t="s">
         <v>314</v>
       </c>
@@ -6813,7 +6838,7 @@
     <row r="172" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="65"/>
       <c r="B172" s="69"/>
-      <c r="C172" s="81"/>
+      <c r="C172" s="92"/>
       <c r="D172" s="10" t="s">
         <v>337</v>
       </c>
@@ -6831,7 +6856,7 @@
       </c>
     </row>
     <row r="173" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A173" s="85" t="s">
+      <c r="A173" s="90" t="s">
         <v>26</v>
       </c>
       <c r="B173" s="63" t="s">
@@ -6859,7 +6884,7 @@
       </c>
     </row>
     <row r="174" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A174" s="86"/>
+      <c r="A174" s="91"/>
       <c r="B174" s="63"/>
       <c r="C174" s="59"/>
       <c r="D174" s="10" t="s">
@@ -6879,7 +6904,7 @@
       </c>
     </row>
     <row r="175" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A175" s="86"/>
+      <c r="A175" s="91"/>
       <c r="B175" s="63"/>
       <c r="C175" s="59"/>
       <c r="D175" s="10" t="s">
@@ -6899,7 +6924,7 @@
       </c>
     </row>
     <row r="176" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A176" s="86"/>
+      <c r="A176" s="91"/>
       <c r="B176" s="63"/>
       <c r="C176" s="59"/>
       <c r="D176" s="10" t="s">
@@ -6919,7 +6944,7 @@
       </c>
     </row>
     <row r="177" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A177" s="86"/>
+      <c r="A177" s="91"/>
       <c r="B177" s="63"/>
       <c r="C177" s="58" t="s">
         <v>321</v>
@@ -6943,7 +6968,7 @@
       </c>
     </row>
     <row r="178" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A178" s="86"/>
+      <c r="A178" s="91"/>
       <c r="B178" s="63"/>
       <c r="C178" s="59"/>
       <c r="D178" s="10" t="s">
@@ -6963,7 +6988,7 @@
       </c>
     </row>
     <row r="179" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A179" s="86"/>
+      <c r="A179" s="91"/>
       <c r="B179" s="63"/>
       <c r="C179" s="59"/>
       <c r="D179" s="10" t="s">
@@ -6983,7 +7008,7 @@
       </c>
     </row>
     <row r="180" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A180" s="86"/>
+      <c r="A180" s="91"/>
       <c r="B180" s="63"/>
       <c r="C180" s="59"/>
       <c r="D180" s="10" t="s">
@@ -7003,7 +7028,7 @@
       </c>
     </row>
     <row r="181" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A181" s="86"/>
+      <c r="A181" s="91"/>
       <c r="B181" s="63"/>
       <c r="C181" s="62" t="s">
         <v>322</v>
@@ -7027,7 +7052,7 @@
       </c>
     </row>
     <row r="182" spans="1:10" s="13" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A182" s="86"/>
+      <c r="A182" s="91"/>
       <c r="B182" s="63"/>
       <c r="C182" s="62"/>
       <c r="D182" s="10" t="s">
@@ -7047,7 +7072,7 @@
       </c>
     </row>
     <row r="183" spans="1:10" s="13" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A183" s="86"/>
+      <c r="A183" s="91"/>
       <c r="B183" s="63"/>
       <c r="C183" s="62"/>
       <c r="D183" s="10" t="s">
@@ -7067,7 +7092,7 @@
       </c>
     </row>
     <row r="184" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A184" s="86"/>
+      <c r="A184" s="91"/>
       <c r="B184" s="63"/>
       <c r="C184" s="62"/>
       <c r="D184" s="10" t="s">
@@ -7087,9 +7112,9 @@
       </c>
     </row>
     <row r="185" spans="1:10" s="13" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A185" s="86"/>
+      <c r="A185" s="91"/>
       <c r="B185" s="63"/>
-      <c r="C185" s="87" t="s">
+      <c r="C185" s="93" t="s">
         <v>323</v>
       </c>
       <c r="D185" s="10" t="s">
@@ -7111,9 +7136,9 @@
       </c>
     </row>
     <row r="186" spans="1:10" s="13" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A186" s="86"/>
+      <c r="A186" s="91"/>
       <c r="B186" s="63"/>
-      <c r="C186" s="88"/>
+      <c r="C186" s="94"/>
       <c r="D186" s="10" t="s">
         <v>224</v>
       </c>
@@ -7131,9 +7156,9 @@
       </c>
     </row>
     <row r="187" spans="1:10" s="13" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A187" s="86"/>
+      <c r="A187" s="91"/>
       <c r="B187" s="63"/>
-      <c r="C187" s="88"/>
+      <c r="C187" s="94"/>
       <c r="D187" s="10" t="s">
         <v>225</v>
       </c>
@@ -7151,9 +7176,9 @@
       </c>
     </row>
     <row r="188" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A188" s="86"/>
+      <c r="A188" s="91"/>
       <c r="B188" s="63"/>
-      <c r="C188" s="89"/>
+      <c r="C188" s="95"/>
       <c r="D188" s="10" t="s">
         <v>226</v>
       </c>
@@ -7177,7 +7202,7 @@
       <c r="B189" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="C189" s="117" t="s">
+      <c r="C189" s="81" t="s">
         <v>324</v>
       </c>
       <c r="D189" s="10" t="s">
@@ -7201,7 +7226,7 @@
     <row r="190" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="65"/>
       <c r="B190" s="69"/>
-      <c r="C190" s="118"/>
+      <c r="C190" s="82"/>
       <c r="D190" s="10" t="s">
         <v>228</v>
       </c>
@@ -7221,7 +7246,7 @@
     <row r="191" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="65"/>
       <c r="B191" s="69"/>
-      <c r="C191" s="118"/>
+      <c r="C191" s="82"/>
       <c r="D191" s="10" t="s">
         <v>229</v>
       </c>
@@ -7241,7 +7266,7 @@
     <row r="192" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="65"/>
       <c r="B192" s="69"/>
-      <c r="C192" s="118"/>
+      <c r="C192" s="82"/>
       <c r="D192" s="10" t="s">
         <v>230</v>
       </c>
@@ -7261,7 +7286,7 @@
     <row r="193" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="65"/>
       <c r="B193" s="69"/>
-      <c r="C193" s="117" t="s">
+      <c r="C193" s="81" t="s">
         <v>325</v>
       </c>
       <c r="D193" s="10" t="s">
@@ -7285,7 +7310,7 @@
     <row r="194" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="65"/>
       <c r="B194" s="69"/>
-      <c r="C194" s="118"/>
+      <c r="C194" s="82"/>
       <c r="D194" s="10" t="s">
         <v>232</v>
       </c>
@@ -7305,7 +7330,7 @@
     <row r="195" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="65"/>
       <c r="B195" s="69"/>
-      <c r="C195" s="118"/>
+      <c r="C195" s="82"/>
       <c r="D195" s="10" t="s">
         <v>233</v>
       </c>
@@ -7325,7 +7350,7 @@
     <row r="196" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="65"/>
       <c r="B196" s="69"/>
-      <c r="C196" s="118"/>
+      <c r="C196" s="82"/>
       <c r="D196" s="10" t="s">
         <v>234</v>
       </c>
@@ -7345,7 +7370,7 @@
     <row r="197" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="65"/>
       <c r="B197" s="69"/>
-      <c r="C197" s="63" t="s">
+      <c r="C197" s="83" t="s">
         <v>326</v>
       </c>
       <c r="D197" s="10" t="s">
@@ -7354,18 +7379,22 @@
       <c r="E197" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="F197" s="60"/>
-      <c r="G197" s="35"/>
-      <c r="H197" s="33"/>
-      <c r="I197" s="33"/>
-      <c r="J197" s="34">
-        <v>0</v>
+      <c r="F197" s="60">
+        <v>0.3</v>
+      </c>
+      <c r="G197" s="46"/>
+      <c r="H197" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I197" s="30"/>
+      <c r="J197" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="198" spans="1:10" s="13" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="65"/>
       <c r="B198" s="69"/>
-      <c r="C198" s="63"/>
+      <c r="C198" s="83"/>
       <c r="D198" s="10" t="s">
         <v>236</v>
       </c>
@@ -7373,17 +7402,19 @@
         <v>463</v>
       </c>
       <c r="F198" s="60"/>
-      <c r="G198" s="35"/>
-      <c r="H198" s="33"/>
-      <c r="I198" s="33"/>
-      <c r="J198" s="34">
-        <v>0</v>
+      <c r="G198" s="46"/>
+      <c r="H198" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I198" s="30"/>
+      <c r="J198" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="199" spans="1:10" s="13" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="65"/>
       <c r="B199" s="69"/>
-      <c r="C199" s="63"/>
+      <c r="C199" s="83"/>
       <c r="D199" s="10" t="s">
         <v>240</v>
       </c>
@@ -7391,17 +7422,19 @@
         <v>466</v>
       </c>
       <c r="F199" s="60"/>
-      <c r="G199" s="35"/>
-      <c r="H199" s="33"/>
-      <c r="I199" s="33"/>
-      <c r="J199" s="34">
-        <v>0</v>
+      <c r="G199" s="46"/>
+      <c r="H199" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I199" s="30"/>
+      <c r="J199" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="200" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="65"/>
       <c r="B200" s="69"/>
-      <c r="C200" s="63"/>
+      <c r="C200" s="83"/>
       <c r="D200" s="10" t="s">
         <v>241</v>
       </c>
@@ -7409,17 +7442,19 @@
         <v>465</v>
       </c>
       <c r="F200" s="60"/>
-      <c r="G200" s="35"/>
-      <c r="H200" s="33"/>
-      <c r="I200" s="33"/>
-      <c r="J200" s="34">
-        <v>0</v>
+      <c r="G200" s="8"/>
+      <c r="H200" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I200" s="30"/>
+      <c r="J200" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="201" spans="1:10" s="13" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="65"/>
       <c r="B201" s="69"/>
-      <c r="C201" s="78" t="s">
+      <c r="C201" s="84" t="s">
         <v>327</v>
       </c>
       <c r="D201" s="10" t="s">
@@ -7428,66 +7463,76 @@
       <c r="E201" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="F201" s="82"/>
-      <c r="G201" s="35"/>
-      <c r="H201" s="33"/>
-      <c r="I201" s="33"/>
-      <c r="J201" s="34">
-        <v>0</v>
+      <c r="F201" s="87">
+        <v>0.2</v>
+      </c>
+      <c r="G201" s="46"/>
+      <c r="H201" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I201" s="30"/>
+      <c r="J201" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="202" spans="1:10" s="13" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="65"/>
       <c r="B202" s="69"/>
-      <c r="C202" s="79"/>
+      <c r="C202" s="85"/>
       <c r="D202" s="10" t="s">
         <v>243</v>
       </c>
       <c r="E202" s="21" t="s">
         <v>463</v>
       </c>
-      <c r="F202" s="83"/>
-      <c r="G202" s="35"/>
-      <c r="H202" s="33"/>
-      <c r="I202" s="33"/>
-      <c r="J202" s="34">
-        <v>0</v>
+      <c r="F202" s="88"/>
+      <c r="G202" s="46"/>
+      <c r="H202" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I202" s="30"/>
+      <c r="J202" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="203" spans="1:10" s="13" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="65"/>
       <c r="B203" s="69"/>
-      <c r="C203" s="79"/>
+      <c r="C203" s="85"/>
       <c r="D203" s="10" t="s">
         <v>244</v>
       </c>
       <c r="E203" s="21" t="s">
         <v>466</v>
       </c>
-      <c r="F203" s="83"/>
-      <c r="G203" s="35"/>
-      <c r="H203" s="33"/>
-      <c r="I203" s="33"/>
-      <c r="J203" s="34">
-        <v>0</v>
+      <c r="F203" s="88"/>
+      <c r="G203" s="46"/>
+      <c r="H203" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I203" s="30"/>
+      <c r="J203" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="204" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="65"/>
-      <c r="B204" s="90"/>
-      <c r="C204" s="81"/>
+      <c r="B204" s="96"/>
+      <c r="C204" s="86"/>
       <c r="D204" s="10" t="s">
         <v>245</v>
       </c>
       <c r="E204" s="21" t="s">
         <v>465</v>
       </c>
-      <c r="F204" s="84"/>
-      <c r="G204" s="35"/>
-      <c r="H204" s="33"/>
-      <c r="I204" s="33"/>
-      <c r="J204" s="34">
-        <v>0</v>
+      <c r="F204" s="89"/>
+      <c r="G204" s="46"/>
+      <c r="H204" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I204" s="30"/>
+      <c r="J204" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="205" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7497,7 +7542,7 @@
       <c r="B205" s="68" t="s">
         <v>184</v>
       </c>
-      <c r="C205" s="66" t="s">
+      <c r="C205" s="123" t="s">
         <v>328</v>
       </c>
       <c r="D205" s="10" t="s">
@@ -7506,18 +7551,22 @@
       <c r="E205" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="F205" s="60"/>
-      <c r="G205" s="38"/>
-      <c r="H205" s="33"/>
-      <c r="I205" s="33"/>
-      <c r="J205" s="34">
-        <v>0</v>
+      <c r="F205" s="60">
+        <v>0.5</v>
+      </c>
+      <c r="G205" s="8"/>
+      <c r="H205" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I205" s="30"/>
+      <c r="J205" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="206" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="65"/>
       <c r="B206" s="69"/>
-      <c r="C206" s="67"/>
+      <c r="C206" s="124"/>
       <c r="D206" s="10" t="s">
         <v>247</v>
       </c>
@@ -7525,17 +7574,19 @@
         <v>463</v>
       </c>
       <c r="F206" s="60"/>
-      <c r="G206" s="37"/>
-      <c r="H206" s="33"/>
-      <c r="I206" s="33"/>
-      <c r="J206" s="34">
-        <v>0</v>
+      <c r="G206" s="9"/>
+      <c r="H206" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I206" s="30"/>
+      <c r="J206" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="207" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="65"/>
       <c r="B207" s="69"/>
-      <c r="C207" s="67"/>
+      <c r="C207" s="124"/>
       <c r="D207" s="10" t="s">
         <v>248</v>
       </c>
@@ -7543,17 +7594,19 @@
         <v>466</v>
       </c>
       <c r="F207" s="60"/>
-      <c r="G207" s="37"/>
-      <c r="H207" s="33"/>
-      <c r="I207" s="33"/>
-      <c r="J207" s="34">
-        <v>0</v>
+      <c r="G207" s="46"/>
+      <c r="H207" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I207" s="30"/>
+      <c r="J207" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="208" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="65"/>
       <c r="B208" s="69"/>
-      <c r="C208" s="67"/>
+      <c r="C208" s="124"/>
       <c r="D208" s="10" t="s">
         <v>249</v>
       </c>
@@ -7561,17 +7614,19 @@
         <v>465</v>
       </c>
       <c r="F208" s="60"/>
-      <c r="G208" s="37"/>
-      <c r="H208" s="33"/>
-      <c r="I208" s="33"/>
-      <c r="J208" s="34">
-        <v>0</v>
+      <c r="G208" s="46"/>
+      <c r="H208" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I208" s="30"/>
+      <c r="J208" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="209" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="65"/>
       <c r="B209" s="69"/>
-      <c r="C209" s="66" t="s">
+      <c r="C209" s="123" t="s">
         <v>329</v>
       </c>
       <c r="D209" s="10" t="s">
@@ -7580,18 +7635,22 @@
       <c r="E209" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="F209" s="60"/>
-      <c r="G209" s="38"/>
-      <c r="H209" s="33"/>
-      <c r="I209" s="33"/>
-      <c r="J209" s="34">
-        <v>0</v>
+      <c r="F209" s="60">
+        <v>0.6</v>
+      </c>
+      <c r="G209" s="8"/>
+      <c r="H209" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I209" s="30"/>
+      <c r="J209" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="210" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="65"/>
       <c r="B210" s="69"/>
-      <c r="C210" s="67"/>
+      <c r="C210" s="124"/>
       <c r="D210" s="10" t="s">
         <v>251</v>
       </c>
@@ -7599,17 +7658,19 @@
         <v>463</v>
       </c>
       <c r="F210" s="60"/>
-      <c r="G210" s="37"/>
-      <c r="H210" s="33"/>
-      <c r="I210" s="33"/>
-      <c r="J210" s="34">
-        <v>0</v>
+      <c r="G210" s="9"/>
+      <c r="H210" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I210" s="30"/>
+      <c r="J210" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="211" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="65"/>
       <c r="B211" s="69"/>
-      <c r="C211" s="67"/>
+      <c r="C211" s="124"/>
       <c r="D211" s="10" t="s">
         <v>258</v>
       </c>
@@ -7617,17 +7678,19 @@
         <v>466</v>
       </c>
       <c r="F211" s="60"/>
-      <c r="G211" s="37"/>
-      <c r="H211" s="33"/>
-      <c r="I211" s="33"/>
-      <c r="J211" s="34">
-        <v>0</v>
+      <c r="G211" s="8"/>
+      <c r="H211" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I211" s="30"/>
+      <c r="J211" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="212" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="65"/>
       <c r="B212" s="69"/>
-      <c r="C212" s="67"/>
+      <c r="C212" s="124"/>
       <c r="D212" s="10" t="s">
         <v>259</v>
       </c>
@@ -7635,17 +7698,19 @@
         <v>465</v>
       </c>
       <c r="F212" s="60"/>
-      <c r="G212" s="37"/>
-      <c r="H212" s="33"/>
-      <c r="I212" s="33"/>
-      <c r="J212" s="34">
-        <v>0</v>
+      <c r="G212" s="46"/>
+      <c r="H212" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I212" s="30"/>
+      <c r="J212" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="213" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="65"/>
       <c r="B213" s="69"/>
-      <c r="C213" s="63" t="s">
+      <c r="C213" s="125" t="s">
         <v>330</v>
       </c>
       <c r="D213" s="10" t="s">
@@ -7654,18 +7719,22 @@
       <c r="E213" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="F213" s="60"/>
-      <c r="G213" s="35"/>
-      <c r="H213" s="33"/>
-      <c r="I213" s="33"/>
-      <c r="J213" s="34">
-        <v>0</v>
+      <c r="F213" s="60">
+        <v>0.5</v>
+      </c>
+      <c r="G213" s="46"/>
+      <c r="H213" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I213" s="30"/>
+      <c r="J213" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="214" spans="1:10" s="13" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="65"/>
       <c r="B214" s="69"/>
-      <c r="C214" s="63"/>
+      <c r="C214" s="125"/>
       <c r="D214" s="10" t="s">
         <v>261</v>
       </c>
@@ -7673,17 +7742,19 @@
         <v>463</v>
       </c>
       <c r="F214" s="60"/>
-      <c r="G214" s="35"/>
-      <c r="H214" s="33"/>
-      <c r="I214" s="33"/>
-      <c r="J214" s="34">
-        <v>0</v>
+      <c r="G214" s="46"/>
+      <c r="H214" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I214" s="30"/>
+      <c r="J214" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="215" spans="1:10" s="13" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="65"/>
       <c r="B215" s="69"/>
-      <c r="C215" s="63"/>
+      <c r="C215" s="125"/>
       <c r="D215" s="10" t="s">
         <v>262</v>
       </c>
@@ -7691,17 +7762,19 @@
         <v>466</v>
       </c>
       <c r="F215" s="60"/>
-      <c r="G215" s="35"/>
-      <c r="H215" s="33"/>
-      <c r="I215" s="33"/>
-      <c r="J215" s="34">
-        <v>0</v>
+      <c r="G215" s="46"/>
+      <c r="H215" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I215" s="30"/>
+      <c r="J215" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="216" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="65"/>
       <c r="B216" s="69"/>
-      <c r="C216" s="63"/>
+      <c r="C216" s="125"/>
       <c r="D216" s="10" t="s">
         <v>263</v>
       </c>
@@ -7709,11 +7782,13 @@
         <v>465</v>
       </c>
       <c r="F216" s="60"/>
-      <c r="G216" s="35"/>
-      <c r="H216" s="33"/>
-      <c r="I216" s="33"/>
-      <c r="J216" s="34">
-        <v>0</v>
+      <c r="G216" s="8"/>
+      <c r="H216" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I216" s="30"/>
+      <c r="J216" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="217" spans="1:10" s="13" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7728,12 +7803,16 @@
       <c r="E217" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="F217" s="60"/>
-      <c r="G217" s="35"/>
-      <c r="H217" s="33"/>
-      <c r="I217" s="33"/>
-      <c r="J217" s="34">
-        <v>0</v>
+      <c r="F217" s="60">
+        <v>0.1</v>
+      </c>
+      <c r="G217" s="46"/>
+      <c r="H217" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I217" s="30"/>
+      <c r="J217" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="218" spans="1:10" s="13" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7747,11 +7826,13 @@
         <v>463</v>
       </c>
       <c r="F218" s="60"/>
-      <c r="G218" s="35"/>
-      <c r="H218" s="33"/>
-      <c r="I218" s="33"/>
-      <c r="J218" s="34">
-        <v>0</v>
+      <c r="G218" s="46"/>
+      <c r="H218" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I218" s="30"/>
+      <c r="J218" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="219" spans="1:10" s="13" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7765,17 +7846,19 @@
         <v>466</v>
       </c>
       <c r="F219" s="60"/>
-      <c r="G219" s="35"/>
-      <c r="H219" s="33"/>
-      <c r="I219" s="33"/>
-      <c r="J219" s="34">
-        <v>0</v>
+      <c r="G219" s="46"/>
+      <c r="H219" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I219" s="30"/>
+      <c r="J219" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="220" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="65"/>
-      <c r="B220" s="90"/>
-      <c r="C220" s="81"/>
+      <c r="B220" s="96"/>
+      <c r="C220" s="92"/>
       <c r="D220" s="10" t="s">
         <v>267</v>
       </c>
@@ -7783,11 +7866,13 @@
         <v>465</v>
       </c>
       <c r="F220" s="60"/>
-      <c r="G220" s="35"/>
-      <c r="H220" s="33"/>
-      <c r="I220" s="33"/>
-      <c r="J220" s="34">
-        <v>0</v>
+      <c r="G220" s="46"/>
+      <c r="H220" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I220" s="30"/>
+      <c r="J220" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="221" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7806,12 +7891,16 @@
       <c r="E221" s="21" t="s">
         <v>464</v>
       </c>
-      <c r="F221" s="60"/>
-      <c r="G221" s="38"/>
-      <c r="H221" s="33"/>
-      <c r="I221" s="33"/>
-      <c r="J221" s="34">
-        <v>0</v>
+      <c r="F221" s="60">
+        <v>0.3</v>
+      </c>
+      <c r="G221" s="8"/>
+      <c r="H221" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I221" s="30"/>
+      <c r="J221" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="222" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7825,11 +7914,13 @@
         <v>463</v>
       </c>
       <c r="F222" s="60"/>
-      <c r="G222" s="37"/>
-      <c r="H222" s="33"/>
-      <c r="I222" s="33"/>
-      <c r="J222" s="34">
-        <v>0</v>
+      <c r="G222" s="46"/>
+      <c r="H222" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I222" s="30"/>
+      <c r="J222" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="223" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7843,11 +7934,13 @@
         <v>466</v>
       </c>
       <c r="F223" s="60"/>
-      <c r="G223" s="37"/>
-      <c r="H223" s="33"/>
-      <c r="I223" s="33"/>
-      <c r="J223" s="34">
-        <v>0</v>
+      <c r="G223" s="46"/>
+      <c r="H223" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I223" s="30"/>
+      <c r="J223" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="224" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7861,11 +7954,13 @@
         <v>465</v>
       </c>
       <c r="F224" s="60"/>
-      <c r="G224" s="37"/>
-      <c r="H224" s="33"/>
-      <c r="I224" s="33"/>
-      <c r="J224" s="34">
-        <v>0</v>
+      <c r="G224" s="46"/>
+      <c r="H224" s="30">
+        <v>43320</v>
+      </c>
+      <c r="I224" s="30"/>
+      <c r="J224" s="31">
+        <v>1</v>
       </c>
     </row>
     <row r="225" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8137,7 +8232,7 @@
         <f>AVERAGE(J241:J304)</f>
         <v>0</v>
       </c>
-      <c r="K238" s="112">
+      <c r="K238" s="118">
         <f>SUM(F241:F304)</f>
         <v>0</v>
       </c>
@@ -8156,7 +8251,7 @@
       <c r="H239" s="55"/>
       <c r="I239" s="55"/>
       <c r="J239" s="57"/>
-      <c r="K239" s="112"/>
+      <c r="K239" s="118"/>
       <c r="L239" s="14"/>
       <c r="M239" s="14"/>
       <c r="N239" s="14"/>
@@ -8477,8 +8572,8 @@
     </row>
     <row r="256" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A256" s="65"/>
-      <c r="B256" s="90"/>
-      <c r="C256" s="81"/>
+      <c r="B256" s="96"/>
+      <c r="C256" s="92"/>
       <c r="D256" s="10" t="s">
         <v>366</v>
       </c>
@@ -8520,7 +8615,7 @@
     <row r="258" spans="1:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="64"/>
       <c r="B258" s="69"/>
-      <c r="C258" s="96"/>
+      <c r="C258" s="102"/>
       <c r="D258" s="10" t="s">
         <v>368</v>
       </c>
@@ -8538,7 +8633,7 @@
     <row r="259" spans="1:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="64"/>
       <c r="B259" s="69"/>
-      <c r="C259" s="96"/>
+      <c r="C259" s="102"/>
       <c r="D259" s="10" t="s">
         <v>369</v>
       </c>
@@ -8556,7 +8651,7 @@
     <row r="260" spans="1:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A260" s="64"/>
       <c r="B260" s="69"/>
-      <c r="C260" s="96"/>
+      <c r="C260" s="102"/>
       <c r="D260" s="10" t="s">
         <v>370</v>
       </c>
@@ -8594,7 +8689,7 @@
     <row r="262" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A262" s="65"/>
       <c r="B262" s="69"/>
-      <c r="C262" s="94"/>
+      <c r="C262" s="100"/>
       <c r="D262" s="20" t="s">
         <v>372</v>
       </c>
@@ -8612,7 +8707,7 @@
     <row r="263" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A263" s="65"/>
       <c r="B263" s="69"/>
-      <c r="C263" s="94"/>
+      <c r="C263" s="100"/>
       <c r="D263" s="20" t="s">
         <v>373</v>
       </c>
@@ -8630,7 +8725,7 @@
     <row r="264" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A264" s="65"/>
       <c r="B264" s="69"/>
-      <c r="C264" s="94"/>
+      <c r="C264" s="100"/>
       <c r="D264" s="20" t="s">
         <v>374</v>
       </c>
@@ -8652,7 +8747,7 @@
       <c r="B265" s="63" t="s">
         <v>384</v>
       </c>
-      <c r="C265" s="113" t="s">
+      <c r="C265" s="119" t="s">
         <v>385</v>
       </c>
       <c r="D265" s="20" t="s">
@@ -8672,7 +8767,7 @@
     <row r="266" spans="1:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A266" s="73"/>
       <c r="B266" s="63"/>
-      <c r="C266" s="114"/>
+      <c r="C266" s="120"/>
       <c r="D266" s="20" t="s">
         <v>376</v>
       </c>
@@ -8690,7 +8785,7 @@
     <row r="267" spans="1:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A267" s="73"/>
       <c r="B267" s="63"/>
-      <c r="C267" s="114"/>
+      <c r="C267" s="120"/>
       <c r="D267" s="20" t="s">
         <v>377</v>
       </c>
@@ -8708,7 +8803,7 @@
     <row r="268" spans="1:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A268" s="73"/>
       <c r="B268" s="63"/>
-      <c r="C268" s="115"/>
+      <c r="C268" s="121"/>
       <c r="D268" s="20" t="s">
         <v>378</v>
       </c>
@@ -8874,7 +8969,7 @@
     <row r="277" spans="1:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A277" s="73"/>
       <c r="B277" s="63"/>
-      <c r="C277" s="87" t="s">
+      <c r="C277" s="93" t="s">
         <v>395</v>
       </c>
       <c r="D277" s="20" t="s">
@@ -8894,7 +8989,7 @@
     <row r="278" spans="1:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A278" s="73"/>
       <c r="B278" s="63"/>
-      <c r="C278" s="88"/>
+      <c r="C278" s="94"/>
       <c r="D278" s="20" t="s">
         <v>398</v>
       </c>
@@ -8912,7 +9007,7 @@
     <row r="279" spans="1:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A279" s="73"/>
       <c r="B279" s="63"/>
-      <c r="C279" s="88"/>
+      <c r="C279" s="94"/>
       <c r="D279" s="20" t="s">
         <v>399</v>
       </c>
@@ -8930,7 +9025,7 @@
     <row r="280" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A280" s="73"/>
       <c r="B280" s="63"/>
-      <c r="C280" s="116"/>
+      <c r="C280" s="122"/>
       <c r="D280" s="20" t="s">
         <v>400</v>
       </c>
@@ -9026,7 +9121,7 @@
       <c r="B285" s="75" t="s">
         <v>407</v>
       </c>
-      <c r="C285" s="95" t="s">
+      <c r="C285" s="101" t="s">
         <v>413</v>
       </c>
       <c r="D285" s="20" t="s">
@@ -9046,7 +9141,7 @@
     <row r="286" spans="1:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A286" s="64"/>
       <c r="B286" s="76"/>
-      <c r="C286" s="96"/>
+      <c r="C286" s="102"/>
       <c r="D286" s="20" t="s">
         <v>409</v>
       </c>
@@ -9064,7 +9159,7 @@
     <row r="287" spans="1:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A287" s="64"/>
       <c r="B287" s="76"/>
-      <c r="C287" s="96"/>
+      <c r="C287" s="102"/>
       <c r="D287" s="20" t="s">
         <v>410</v>
       </c>
@@ -9082,7 +9177,7 @@
     <row r="288" spans="1:10" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A288" s="64"/>
       <c r="B288" s="76"/>
-      <c r="C288" s="96"/>
+      <c r="C288" s="102"/>
       <c r="D288" s="20" t="s">
         <v>411</v>
       </c>
@@ -9440,7 +9535,7 @@
         <f>AVERAGE(J309:J332)</f>
         <v>0</v>
       </c>
-      <c r="K306" s="112">
+      <c r="K306" s="118">
         <f>SUM(F309:F332)</f>
         <v>0</v>
       </c>
@@ -9459,7 +9554,7 @@
       <c r="H307" s="55"/>
       <c r="I307" s="55"/>
       <c r="J307" s="57"/>
-      <c r="K307" s="112"/>
+      <c r="K307" s="118"/>
       <c r="L307" s="14"/>
       <c r="M307" s="14"/>
     </row>
@@ -9496,7 +9591,7 @@
       </c>
     </row>
     <row r="309" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A309" s="97" t="s">
+      <c r="A309" s="103" t="s">
         <v>32</v>
       </c>
       <c r="B309" s="66" t="s">
@@ -9520,9 +9615,9 @@
       </c>
     </row>
     <row r="310" spans="1:14" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A310" s="98"/>
-      <c r="B310" s="96"/>
-      <c r="C310" s="96"/>
+      <c r="A310" s="104"/>
+      <c r="B310" s="102"/>
+      <c r="C310" s="102"/>
       <c r="D310" s="10" t="s">
         <v>434</v>
       </c>
@@ -9538,9 +9633,9 @@
       </c>
     </row>
     <row r="311" spans="1:14" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A311" s="98"/>
-      <c r="B311" s="96"/>
-      <c r="C311" s="96"/>
+      <c r="A311" s="104"/>
+      <c r="B311" s="102"/>
+      <c r="C311" s="102"/>
       <c r="D311" s="10" t="s">
         <v>435</v>
       </c>
@@ -9556,7 +9651,7 @@
       </c>
     </row>
     <row r="312" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A312" s="99"/>
+      <c r="A312" s="105"/>
       <c r="B312" s="67"/>
       <c r="C312" s="67"/>
       <c r="D312" s="10" t="s">
@@ -9994,7 +10089,7 @@
         <f>AVERAGE(J337:J354)</f>
         <v>0</v>
       </c>
-      <c r="K334" s="112">
+      <c r="K334" s="118">
         <f>SUM(F337:F354)</f>
         <v>0</v>
       </c>
@@ -10013,7 +10108,7 @@
       <c r="H335" s="55"/>
       <c r="I335" s="55"/>
       <c r="J335" s="57"/>
-      <c r="K335" s="112"/>
+      <c r="K335" s="118"/>
       <c r="L335" s="14"/>
       <c r="M335" s="14"/>
     </row>

</xml_diff>